<commit_message>
Fixat New Car Brand/Model och design
</commit_message>
<xml_diff>
--- a/Scheman-Dokument/Testplan Miniprojekt Bilmärken (1).xlsx
+++ b/Scheman-Dokument/Testplan Miniprojekt Bilmärken (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TildeFagerström\Documents\GitHub\Windowsprogrammering-Miniprojekt\Scheman-Dokument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B9E4A7-39D8-428B-908C-8D93B7E2DDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0EA563-8ECF-4B58-AB4F-1F84F14B54C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8179A04-2F19-43BA-94ED-4240E42F7E58}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Testplan</t>
   </si>
@@ -135,6 +135,21 @@
   </si>
   <si>
     <t>Ja</t>
+  </si>
+  <si>
+    <t>New Car Brand knappen</t>
+  </si>
+  <si>
+    <t>Se till att man kan skriva in i nytt land rutan och att knapparna är synliga när de ska</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>New Car Model fönster dyker upp</t>
+  </si>
+  <si>
+    <t>Man kan skriva in en ny bilmodell</t>
   </si>
 </sst>
 </file>
@@ -768,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C14B1C6-3F39-49A4-A27F-26B97EB4A65C}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,16 +794,17 @@
     <col min="1" max="1" width="118.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="15"/>
     </row>
-    <row r="2" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -799,7 +815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -810,25 +826,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -836,8 +862,14 @@
       <c r="C6" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -845,8 +877,11 @@
       <c r="C7" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -854,8 +889,11 @@
       <c r="C8" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -864,7 +902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -873,7 +911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -882,7 +920,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -891,7 +929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -900,7 +938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -909,7 +947,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -918,7 +956,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Fixat i testplanen och gjort klart frmarna
</commit_message>
<xml_diff>
--- a/Scheman-Dokument/Testplan Miniprojekt Bilmärken (1).xlsx
+++ b/Scheman-Dokument/Testplan Miniprojekt Bilmärken (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TildeFagerström\Documents\GitHub\Windowsprogrammering-Miniprojekt\Scheman-Dokument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0EA563-8ECF-4B58-AB4F-1F84F14B54C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782FAB4B-E37B-42F1-8FDA-8EF43F3F0F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8179A04-2F19-43BA-94ED-4240E42F7E58}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>Testplan</t>
   </si>
@@ -150,6 +150,39 @@
   </si>
   <si>
     <t>Man kan skriva in en ny bilmodell</t>
+  </si>
+  <si>
+    <t>databasen uppdateras</t>
+  </si>
+  <si>
+    <t>Databasen uppdateras när man lägger till ett bilmärke</t>
+  </si>
+  <si>
+    <t>Databasen uppdateras när man lägger till ett land</t>
+  </si>
+  <si>
+    <t>Man kan ta bort ett land från listan</t>
+  </si>
+  <si>
+    <t>Landet försvinner från databasen om man raderar det</t>
+  </si>
+  <si>
+    <t>Man får upp en msg box om man vill radera ett land</t>
+  </si>
+  <si>
+    <t>om man klickar "No" på msg boxen kommer man tillbaka</t>
+  </si>
+  <si>
+    <t>nej</t>
+  </si>
+  <si>
+    <t>Test 16: Testa att man bara kan skriva in bokstäver på textrutor för namn osv.</t>
+  </si>
+  <si>
+    <t>textruta kan bara skriva in siffor</t>
+  </si>
+  <si>
+    <t>Test 17: Testa att man bara kan skriva in siffror med en desimal på de textruror som behövs och att det kommer upp en msg box annars</t>
   </si>
 </sst>
 </file>
@@ -436,7 +469,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -465,6 +498,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -783,15 +820,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C14B1C6-3F39-49A4-A27F-26B97EB4A65C}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B2" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="118.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="122.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.28515625" bestFit="1" customWidth="1"/>
@@ -858,7 +895,9 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C6" s="8" t="s">
         <v>22</v>
       </c>
@@ -873,94 +912,162 @@
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C7" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C8" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C9" s="8" t="s">
         <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C10" s="8" t="s">
         <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C11" s="8" t="s">
         <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C12" s="8" t="s">
         <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="C13" s="8" t="s">
         <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C14" s="8" t="s">
         <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C15" s="8" t="s">
         <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C16" s="8" t="s">
         <v>31</v>
       </c>
@@ -969,8 +1076,23 @@
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Fixat i testplanen och gjort klart frmarna och små funktioner
</commit_message>
<xml_diff>
--- a/Scheman-Dokument/Testplan Miniprojekt Bilmärken (1).xlsx
+++ b/Scheman-Dokument/Testplan Miniprojekt Bilmärken (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TildeFagerström\Documents\GitHub\Windowsprogrammering-Miniprojekt\Scheman-Dokument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782FAB4B-E37B-42F1-8FDA-8EF43F3F0F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1618CD6F-3E97-4D0A-AF89-CC2E067A6BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8179A04-2F19-43BA-94ED-4240E42F7E58}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="86">
   <si>
     <t>Testplan</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Test 14: Testa att man kan ändra/ta bort ett land om man klickar på ett land</t>
   </si>
   <si>
-    <t xml:space="preserve">Test 15: Testa att Ändra/Ta bort knappen enbart syns när man klickar på ett land </t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -183,6 +180,120 @@
   </si>
   <si>
     <t>Test 17: Testa att man bara kan skriva in siffror med en desimal på de textruror som behövs och att det kommer upp en msg box annars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 15: Testa att Ändra/Ta bort knappen enbart går att klicka på när man klickar på ett land </t>
+  </si>
+  <si>
+    <t>Testplan - Rapport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 4: Testa att man kan skriva in i nytt land rutan och att knapparna är synliga i de sammanhang det ska vara </t>
+  </si>
+  <si>
+    <t>Nytt land rutan &amp; knappars synlighet</t>
+  </si>
+  <si>
+    <t>Test 5: Testa att man får upp ett nytt formulär när man klickar på nytt bilmärke knappen</t>
+  </si>
+  <si>
+    <t>Test 6: Testa att det dyker upp ett nytt formulär man trycker på Ny bilmodell knappen</t>
+  </si>
+  <si>
+    <t>Ny Bilmodell knapp</t>
+  </si>
+  <si>
+    <t>Test 7: Testa att man kan fylla i en ny bilmodell i fomruläret</t>
+  </si>
+  <si>
+    <t>Fylla i en ny bilmodell</t>
+  </si>
+  <si>
+    <t>Test 8: Testa att databasen uppdateras när man lägger till en ny bilmodell och sparar</t>
+  </si>
+  <si>
+    <t>Uppdatera och spara databasen</t>
+  </si>
+  <si>
+    <t>Test 9: Testa att databasen uppdateras när man lägger till ett nytt bilmärke</t>
+  </si>
+  <si>
+    <t>Uppdatera och spara databasen vid nytt bilmärke</t>
+  </si>
+  <si>
+    <t>Test 10: Testa att databasen uppdateras när man lägger till ett nytt land</t>
+  </si>
+  <si>
+    <t>Uppdatera och spara databasen vid nytt land</t>
+  </si>
+  <si>
+    <t>Test 11: Testa att databasen uppdateras samt listan i trädvyn uppdateras</t>
+  </si>
+  <si>
+    <t>Databasen &amp; trädvyn uppdateras</t>
+  </si>
+  <si>
+    <t>Test 12: Testa att man kan ångra efter man tryckt på "nytt land"</t>
+  </si>
+  <si>
+    <t>Ångra knappen vid nytt land</t>
+  </si>
+  <si>
+    <t>Test 13: Testa att man får upp en drop down lista med alla länder som man kan välja ifrån och att man kan fylla i och spara bilmärke</t>
+  </si>
+  <si>
+    <t>Test 14: Testa att man enbart kan klicka på knappen "Ny bilmodell" när man är inne på ett bilmärke</t>
+  </si>
+  <si>
+    <t>Synlighet för knappen "New Car Model"</t>
+  </si>
+  <si>
+    <t>Test 15: Testa att man kan abryta att fylla i formulären</t>
+  </si>
+  <si>
+    <t>Avbrytar knapparna</t>
+  </si>
+  <si>
+    <t>Test 16: Testa att man kan ändra/ta bort ett land om man klickar på ett land</t>
+  </si>
+  <si>
+    <t>Ta bort/Ändra knappen</t>
+  </si>
+  <si>
+    <t>Test 17: Testa att ett land försvinner om man raderar det &amp; att databasen uppdateras samt trädvyn</t>
+  </si>
+  <si>
+    <t>Ta bort land &amp; uppdatera databas/trädvy</t>
+  </si>
+  <si>
+    <t>Test 18: Testa att man får upp en msg box om man vill radera ett land</t>
+  </si>
+  <si>
+    <t>MSG box</t>
+  </si>
+  <si>
+    <t>Test 19: Testa om man klickar på "No" på msg boxen kommer man tillbaka</t>
+  </si>
+  <si>
+    <t>yes/no formulär</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 20: Testa att Ändra/Ta bort knappen enbart går att klicka på när man klickar på ett land </t>
+  </si>
+  <si>
+    <t>Tillgängligheten på ändra/ta bort knappen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 21: Testa att man bara kan skriva in siffror med en desimal på de textruror som behövs </t>
+  </si>
+  <si>
+    <t>Bara skriva in siffror och en decimal</t>
+  </si>
+  <si>
+    <t>Test 22: Testa att man kan få drop down på motorstorlek och Årsmodell när man ska fylla i formuläret</t>
+  </si>
+  <si>
+    <t>Drop down lista för årsmodell</t>
   </si>
 </sst>
 </file>
@@ -242,7 +353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -458,6 +569,76 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -469,14 +650,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,10 +665,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -500,8 +681,46 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -820,283 +1039,568 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C14B1C6-3F39-49A4-A27F-26B97EB4A65C}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B1048576"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="122.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="122.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+    </row>
+    <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="26" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B26" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="8" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="8" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>48</v>
-      </c>
+      <c r="C37" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="14"/>
+    </row>
+    <row r="47" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="14"/>
+    </row>
+    <row r="48" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="14"/>
+    </row>
+    <row r="49" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Skrivit klart Projektrapporten, fixat diagram och fixat några små saker i Visual Studio
</commit_message>
<xml_diff>
--- a/Scheman-Dokument/Testplan Miniprojekt Bilmärken (1).xlsx
+++ b/Scheman-Dokument/Testplan Miniprojekt Bilmärken (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TildeFagerström\Documents\GitHub\Windowsprogrammering-Miniprojekt\Scheman-Dokument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1618CD6F-3E97-4D0A-AF89-CC2E067A6BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05555035-6725-4DB2-B49A-2782FFBCB869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8179A04-2F19-43BA-94ED-4240E42F7E58}"/>
   </bookViews>
@@ -650,7 +650,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -672,26 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -701,7 +682,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -714,14 +694,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1041,30 +1039,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C14B1C6-3F39-49A4-A27F-26B97EB4A65C}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="122.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -1075,7 +1073,7 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="17" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1086,7 +1084,7 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1097,7 +1095,7 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1114,7 +1112,7 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1131,7 +1129,7 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1148,7 +1146,7 @@
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1165,7 +1163,7 @@
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1182,7 +1180,7 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1199,7 +1197,7 @@
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1216,7 +1214,7 @@
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1233,7 +1231,7 @@
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1250,7 +1248,7 @@
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1267,7 +1265,7 @@
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1284,7 +1282,7 @@
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1295,7 +1293,7 @@
       <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="18" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="6"/>
@@ -1316,31 +1314,31 @@
     <row r="20" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
     </row>
     <row r="23" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="21" t="s">
+      <c r="B24" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1348,7 +1346,7 @@
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1359,7 +1357,7 @@
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1370,7 +1368,7 @@
       <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -1381,7 +1379,7 @@
       <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -1392,7 +1390,7 @@
       <c r="A29" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -1403,7 +1401,7 @@
       <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -1414,7 +1412,7 @@
       <c r="A31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -1425,178 +1423,164 @@
       <c r="A32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="18" t="s">
         <v>34</v>
       </c>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="14"/>
-    </row>
-    <row r="47" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="14"/>
-    </row>
-    <row r="48" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="14"/>
-    </row>
-    <row r="49" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-    </row>
+    <row r="46" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="11"/>
+    </row>
+    <row r="47" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="11"/>
+    </row>
+    <row r="48" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="11"/>
+    </row>
+    <row r="49" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>

</xml_diff>